<commit_message>
feat: auto sending mail project
Summarize input keyword and save excel file
sending e-mail with excel file
</commit_message>
<xml_diff>
--- a/mini_project_3/email list_fastcampus news.xlsx
+++ b/mini_project_3/email list_fastcampus news.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muhn2-008/Documents/dev/KDT_HW/mini_project_3/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B31D7E0-871F-5B47-9C62-BF1B921BDAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-19180" yWindow="1880" windowWidth="17660" windowHeight="12680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="시트1" sheetId="1" r:id="rId4"/>
+    <sheet name="시트1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>email_list</t>
   </si>
@@ -25,9 +34,6 @@
     <t>이메일</t>
   </si>
   <si>
-    <t>배프</t>
-  </si>
-  <si>
     <t>beap.jg@gmail.com</t>
   </si>
   <si>
@@ -131,64 +137,105 @@
   </si>
   <si>
     <t>패스트캠퍼스, 비전문가를 전문가로 키워주는 실무교육 전면 개편 조선비즈언론사 선정 2019.09.25. 네이버뉴스 패스트캠퍼스, 커리어 전환 풀타임 교육 ‘스쿨’ 개편 ZDNet Korea 2019.09.25. 네이버뉴스</t>
+  </si>
+  <si>
+    <t>박강민</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>베프</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>sck04184@naver.com</t>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="11">
-    <font>
-      <sz val="10.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="13">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="&quot;맑은 고딕&quot;"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Arial"/>
-    </font>
-    <font>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font/>
-    <font>
-      <sz val="11.0"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="나눔명조"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="3">
@@ -196,7 +243,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -206,84 +253,72 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
+      <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -473,23 +508,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AE17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="22.71"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:31" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,7 +537,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:31" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -509,48 +549,59 @@
       </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:31" ht="15.75" customHeight="1">
       <c r="A3" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A4" s="8">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="11"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="12" t="s">
-        <v>8</v>
-      </c>
       <c r="B6" s="13"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:31">
       <c r="A7" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="D7" s="14" t="s">
         <v>10</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>11</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
@@ -580,18 +631,18 @@
       <c r="AD7" s="15"/>
       <c r="AE7" s="15"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:31">
       <c r="A8" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="D8" s="14" t="s">
         <v>13</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>14</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
@@ -621,18 +672,18 @@
       <c r="AD8" s="15"/>
       <c r="AE8" s="15"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:31">
       <c r="A9" s="16">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="D9" s="14" t="s">
         <v>16</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>17</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
@@ -662,18 +713,18 @@
       <c r="AD9" s="15"/>
       <c r="AE9" s="15"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:31">
       <c r="A10" s="16">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="D10" s="14" t="s">
         <v>19</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>20</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
@@ -703,18 +754,18 @@
       <c r="AD10" s="15"/>
       <c r="AE10" s="15"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:31">
       <c r="A11" s="16">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="D11" s="14" t="s">
         <v>22</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>23</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
@@ -744,18 +795,18 @@
       <c r="AD11" s="15"/>
       <c r="AE11" s="15"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:31">
       <c r="A12" s="16">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B12" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="D12" s="14" t="s">
         <v>25</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>26</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -785,18 +836,18 @@
       <c r="AD12" s="15"/>
       <c r="AE12" s="15"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:31">
       <c r="A13" s="16">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="D13" s="14" t="s">
         <v>28</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>29</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -826,18 +877,18 @@
       <c r="AD13" s="15"/>
       <c r="AE13" s="15"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:31">
       <c r="A14" s="16">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B14" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="D14" s="14" t="s">
         <v>31</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>32</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -867,18 +918,18 @@
       <c r="AD14" s="15"/>
       <c r="AE14" s="15"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:31">
       <c r="A15" s="16">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>34</v>
-      </c>
       <c r="D15" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -908,18 +959,18 @@
       <c r="AD15" s="15"/>
       <c r="AE15" s="15"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:31">
       <c r="A16" s="16">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B16" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="17" t="s">
-        <v>36</v>
-      </c>
       <c r="D16" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -949,18 +1000,18 @@
       <c r="AD16" s="15"/>
       <c r="AE16" s="15"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:31">
       <c r="A17" s="16">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B17" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="D17" s="14" t="s">
         <v>38</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>39</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -991,20 +1042,22 @@
       <c r="AE17" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C3"/>
-    <hyperlink r:id="rId2" ref="C4"/>
-    <hyperlink r:id="rId3" ref="C8"/>
-    <hyperlink r:id="rId4" ref="C9"/>
-    <hyperlink r:id="rId5" ref="C10"/>
-    <hyperlink r:id="rId6" ref="C11"/>
-    <hyperlink r:id="rId7" ref="C12"/>
-    <hyperlink r:id="rId8" ref="C13"/>
-    <hyperlink r:id="rId9" ref="C14"/>
-    <hyperlink r:id="rId10" ref="C15"/>
-    <hyperlink r:id="rId11" ref="C16"/>
-    <hyperlink r:id="rId12" ref="C17"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C13" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C14" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C15" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C16" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C17" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C5" r:id="rId13" xr:uid="{8DF3D241-B063-A848-BB11-A81AC930BD2C}"/>
   </hyperlinks>
-  <drawing r:id="rId13"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>